<commit_message>
feat: further analysis of max discount
</commit_message>
<xml_diff>
--- a/lab06/ExcelAnalysis.xlsx
+++ b/lab06/ExcelAnalysis.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jantar\uni-data-warehouse\lab06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D8851B-065E-44A9-A22D-3FFDA87E59A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E750113-F218-45CC-8E71-A0D7A2F5F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E48C8BCD-939F-42B2-9A29-188705BE0DA9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{E48C8BCD-939F-42B2-9A29-188705BE0DA9}"/>
   </bookViews>
   <sheets>
     <sheet name="bike sales" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
   <calcPr calcId="0"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="2" r:id="rId5"/>
-    <pivotCache cacheId="8" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="19" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -2286,6 +2286,462 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -8356,16 +8812,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>933449</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>42864</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>71439</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8806,7 +9262,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Jantar" refreshedDate="45781.90054722222" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{AC43C714-3A94-4D24-A523-F366C8B6633A}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Jantar" refreshedDate="45782.484770486109" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{AC43C714-3A94-4D24-A523-F366C8B6633A}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="11">
     <cacheField name="[DIM PRODUCT].[Category Name].[Category Name]" caption="Category Name" numFmtId="0" hierarchy="7" level="1">
@@ -9206,7 +9662,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59E02679-9E90-44E8-B5B9-A2005CF33EBD}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59E02679-9E90-44E8-B5B9-A2005CF33EBD}" name="PivotTable2" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
   <location ref="A4:F10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1"/>
@@ -9433,7 +9889,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0DED4066-AE2E-47FD-8DCC-DCC76D438D76}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="9" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0DED4066-AE2E-47FD-8DCC-DCC76D438D76}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="9" fieldListSortAscending="1">
   <location ref="A4:G29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1"/>
@@ -10321,8 +10777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649D47CE-5CE8-4170-B1D5-EF78E258C8C0}">
   <dimension ref="A4:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10333,11 +10789,11 @@
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>